<commit_message>
Added budget and Type column
</commit_message>
<xml_diff>
--- a/price.xlsx
+++ b/price.xlsx
@@ -5,21 +5,29 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Item</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -30,6 +38,9 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Budget Left</t>
   </si>
   <si>
     <t>Motor</t>
@@ -48,15 +59,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="#.00"/>
+    <numFmt numFmtId="165" formatCode="GENERAL"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -73,13 +86,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,8 +117,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+  <cellStyleXfs count="22">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -115,25 +141,125 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="6">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Untitled1" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#.00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -142,100 +268,122 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.82142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="6.98469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.55102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.98469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <f aca="false">D2*C2</f>
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <f aca="false">SUM(E:E)</f>
+        <v>62</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <f aca="false">SUM(100-(G2))</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <f aca="false">D3*C3</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <f aca="false">D4*C4</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <f aca="false">C2*B2</f>
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <f aca="false">SUM(D2:D5)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="E5" s="2" t="n">
+        <f aca="false">D5*C5</f>
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <f aca="false">C3*B3</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">C4*B4</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">C5*B5</f>
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Design in block form
</commit_message>
<xml_diff>
--- a/price.xlsx
+++ b/price.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Item</t>
   </si>
@@ -31,38 +31,69 @@
     <t>Amount</t>
   </si>
   <si>
+    <t>Extras</t>
+  </si>
+  <si>
     <t>Price ea</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
+    <t>website</t>
+  </si>
+  <si>
     <t>Sum</t>
   </si>
   <si>
     <t>Budget Left</t>
   </si>
   <si>
+    <t>USD 2 HUF</t>
+  </si>
+  <si>
     <t>Motor</t>
   </si>
   <si>
+    <t>http://www.aliexpress.com/item/5V-4-Phase-Stepper-Step-Motor-Driver-Board-ULN2003-for-Arduino/32267738347.html?spm=2114.01010208.3.26.aWne52&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=b59819fd-5edf-4c86-af97-df02f3498318</t>
+  </si>
+  <si>
     <t>Controller</t>
   </si>
   <si>
-    <t>Wifi Module</t>
+    <t>A3967 Microstep driver</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/af/easy-driver-stepper-motor-driver.html?ltype=wholesale&amp;d=y&amp;origin=n&amp;isViewCP=y&amp;catId=0&amp;initiative_id=AS_20160307053856&amp;SearchText=easy+driver+stepper+motor+driver</t>
+  </si>
+  <si>
+    <t>BLE Module</t>
+  </si>
+  <si>
+    <t>http://www.hestore.hu/prod_10026473.html</t>
   </si>
   <si>
     <t>PIR Motion Sensor</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/1pcs-High-Quality-HC-SR501-Infrared-PIR-Motion-Sensor-Module-For-Arduino-Raspberry-pi/32558562655.html?spm=2114.01010208.3.1.Q24Qu6&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=39551360-2e93-4fcf-b607-dc7a7b7ec915</t>
+  </si>
+  <si>
+    <t>PI BLE</t>
+  </si>
+  <si>
+    <t>https://www.pcx.hu/halozat/bluetooth?gclid=CPH2pMTYrssCFUqeGwodtAwACg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#.00"/>
     <numFmt numFmtId="165" formatCode="GENERAL"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ [$HUF];[RED]\-#,##0.00\ [$HUF]"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -88,24 +119,18 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,7 +142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="20">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -141,14 +166,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,32 +176,50 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Untitled1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -268,122 +305,186 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.82142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="35.3316326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
+      <c r="A2" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <f aca="false">D2*C2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <f aca="false">E2*(C2+D2)</f>
+        <v>6.15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <f aca="false">SUM(F:F)</f>
+        <v>64.4843772241993</v>
+      </c>
+      <c r="J2" s="7" t="n">
+        <f aca="false">SUM(100-(I2))</f>
+        <v>35.5156227758007</v>
+      </c>
+      <c r="N2" s="9" t="n">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <f aca="false">SUM(E:E)</f>
-        <v>62</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <f aca="false">SUM(100-(G2))</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <f aca="false">D3*C3</f>
-        <v>10</v>
+      <c r="F3" s="7" t="n">
+        <f aca="false">E3*(C3+D3)</f>
+        <v>20</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
+      <c r="A4" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <f aca="false">D4*C4</f>
-        <v>30</v>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <f aca="false">3201/N2</f>
+        <v>11.3914590747331</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <f aca="false">E4*(C4+D4)</f>
+        <v>34.1743772241993</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
+      <c r="A5" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <f aca="false">D5*C5</f>
-        <v>10</v>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <f aca="false">E5*(C5+D5)</f>
+        <v>4.16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <f aca="false">E6*(C6+D6)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="http://www.aliexpress.com/item/5V-4-Phase-Stepper-Step-Motor-Driver-Board-ULN2003-for-Arduino/32267738347.html?spm=2114.01010208.3.26.aWne52&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=b59819fd-5edf-4c86-af97-df02f3498318"/>
+    <hyperlink ref="G4" r:id="rId2" display="http://www.hestore.hu/prod_10026473.html"/>
+    <hyperlink ref="G5" r:id="rId3" display="http://www.aliexpress.com/item/1pcs-High-Quality-HC-SR501-Infrared-PIR-Motion-Sensor-Module-For-Arduino-Raspberry-pi/32558562655.html?spm=2114.01010208.3.1.Q24Qu6&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=39551360-2e93-4fcf-b607-dc7a7b7ec915"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Need to find usb dogle
</commit_message>
<xml_diff>
--- a/price.xlsx
+++ b/price.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -70,7 +70,7 @@
     <t>BLE Module</t>
   </si>
   <si>
-    <t>http://www.hestore.hu/prod_10026473.html</t>
+    <t>http://www.hestore.hu/prod_10032544.html</t>
   </si>
   <si>
     <t>PIR Motion Sensor</t>
@@ -308,20 +308,23 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="35.3316326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,6 +364,7 @@
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="B2" s="0"/>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
@@ -379,11 +383,11 @@
       </c>
       <c r="I2" s="7" t="n">
         <f aca="false">SUM(F:F)</f>
-        <v>64.4843772241993</v>
+        <v>52.0529181494662</v>
       </c>
       <c r="J2" s="7" t="n">
         <f aca="false">SUM(100-(I2))</f>
-        <v>35.5156227758007</v>
+        <v>47.9470818505338</v>
       </c>
       <c r="N2" s="9" t="n">
         <v>281</v>
@@ -393,7 +397,7 @@
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -418,7 +422,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -429,7 +433,7 @@
       </c>
       <c r="F4" s="7" t="n">
         <f aca="false">E4*(C4+D4)</f>
-        <v>34.1743772241993</v>
+        <v>22.7829181494662</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>16</v>
@@ -440,7 +444,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2</v>
@@ -450,18 +454,18 @@
       </c>
       <c r="F5" s="7" t="n">
         <f aca="false">E5*(C5+D5)</f>
-        <v>4.16</v>
+        <v>3.12</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
@@ -470,7 +474,7 @@
         <f aca="false">E6*(C6+D6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -482,7 +486,7 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="http://www.aliexpress.com/item/5V-4-Phase-Stepper-Step-Motor-Driver-Board-ULN2003-for-Arduino/32267738347.html?spm=2114.01010208.3.26.aWne52&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=b59819fd-5edf-4c86-af97-df02f3498318"/>
-    <hyperlink ref="G4" r:id="rId2" display="http://www.hestore.hu/prod_10026473.html"/>
+    <hyperlink ref="G4" r:id="rId2" display="http://www.hestore.hu/prod_10032544.html"/>
     <hyperlink ref="G5" r:id="rId3" display="http://www.aliexpress.com/item/1pcs-High-Quality-HC-SR501-Infrared-PIR-Motion-Sensor-Module-For-Arduino-Raspberry-pi/32558562655.html?spm=2114.01010208.3.1.Q24Qu6&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=39551360-2e93-4fcf-b607-dc7a7b7ec915"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
hyperlink links changed and cleared, prices updated, all types added
</commit_message>
<xml_diff>
--- a/price.xlsx
+++ b/price.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Item</t>
   </si>
@@ -49,13 +49,16 @@
     <t>Budget Left</t>
   </si>
   <si>
-    <t>USD 2 HUF</t>
+    <t>USD → HUF</t>
   </si>
   <si>
     <t>Motor</t>
   </si>
   <si>
-    <t>http://www.aliexpress.com/item/5V-4-Phase-Stepper-Step-Motor-Driver-Board-ULN2003-for-Arduino/32267738347.html?spm=2114.01010208.3.26.aWne52&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=b59819fd-5edf-4c86-af97-df02f3498318</t>
+    <t>5V 4 phase stepper motor</t>
+  </si>
+  <si>
+    <t>Stepper motor</t>
   </si>
   <si>
     <t>Controller</t>
@@ -64,25 +67,28 @@
     <t>A3967 Microstep driver</t>
   </si>
   <si>
-    <t>http://www.aliexpress.com/af/easy-driver-stepper-motor-driver.html?ltype=wholesale&amp;d=y&amp;origin=n&amp;isViewCP=y&amp;catId=0&amp;initiative_id=AS_20160307053856&amp;SearchText=easy+driver+stepper+motor+driver</t>
+    <t>stepper motor driver search</t>
   </si>
   <si>
     <t>BLE Module</t>
   </si>
   <si>
-    <t>http://www.hestore.hu/prod_10032544.html</t>
+    <t>BTM-800 PRX</t>
   </si>
   <si>
     <t>PIR Motion Sensor</t>
   </si>
   <si>
-    <t>http://www.aliexpress.com/item/1pcs-High-Quality-HC-SR501-Infrared-PIR-Motion-Sensor-Module-For-Arduino-Raspberry-pi/32558562655.html?spm=2114.01010208.3.1.Q24Qu6&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=39551360-2e93-4fcf-b607-dc7a7b7ec915</t>
+    <t>HC-SR501</t>
+  </si>
+  <si>
+    <t>PIR motion sensor</t>
   </si>
   <si>
     <t>PI BLE</t>
   </si>
   <si>
-    <t>https://www.pcx.hu/halozat/bluetooth?gclid=CPH2pMTYrssCFUqeGwodtAwACg</t>
+    <t>PCX ble usb search</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ [$HUF];[RED]\-#,##0.00\ [$HUF]"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,6 +122,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -167,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -176,20 +189,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -200,16 +209,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -305,29 +310,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.37755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.6122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.43367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -346,7 +351,7 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -358,136 +363,151 @@
       <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>2.05</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <f aca="false">E2*(C2+D2)</f>
+      <c r="F3" s="6" t="n">
+        <f aca="false">E3*(C3+D3)</f>
         <v>6.15</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="7" t="n">
+      <c r="G3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="6" t="n">
         <f aca="false">SUM(F:F)</f>
-        <v>52.0529181494662</v>
-      </c>
-      <c r="J2" s="7" t="n">
-        <f aca="false">SUM(100-(I2))</f>
-        <v>47.9470818505338</v>
-      </c>
-      <c r="N2" s="9" t="n">
+        <v>52.5137722419929</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <f aca="false">SUM(100-(I3))</f>
+        <v>47.4862277580071</v>
+      </c>
+      <c r="N3" s="8" t="n">
         <v>281</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <f aca="false">E3*(C3+D3)</f>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <f aca="false">E4*(C4+D4)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <f aca="false">5303/N3</f>
+        <v>18.8718861209964</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <f aca="false">E5*(C5+D5)</f>
+        <v>37.7437722419929</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <f aca="false">E6*(C6+D6)</f>
+        <v>3.12</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <f aca="false">3201/N2</f>
-        <v>11.3914590747331</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <f aca="false">E4*(C4+D4)</f>
-        <v>22.7829181494662</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <f aca="false">E5*(C5+D5)</f>
-        <v>3.12</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="n">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <f aca="false">E7*(C7+D7)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="7" t="n">
-        <f aca="false">E6*(C6+D6)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>20</v>
+      <c r="G7" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J3">
     <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="http://www.aliexpress.com/item/5V-4-Phase-Stepper-Step-Motor-Driver-Board-ULN2003-for-Arduino/32267738347.html?spm=2114.01010208.3.26.aWne52&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=b59819fd-5edf-4c86-af97-df02f3498318"/>
-    <hyperlink ref="G4" r:id="rId2" display="http://www.hestore.hu/prod_10032544.html"/>
-    <hyperlink ref="G5" r:id="rId3" display="http://www.aliexpress.com/item/1pcs-High-Quality-HC-SR501-Infrared-PIR-Motion-Sensor-Module-For-Arduino-Raspberry-pi/32558562655.html?spm=2114.01010208.3.1.Q24Qu6&amp;ws_ab_test=searchweb201556_7,searchweb201644_3_505_506_503_504_301_10020_502_10001_10002_10017_10005_10006_10003_10021_10004_10022_10018_10019,searchweb201560_8,searchweb1451318400_-1,searchweb1451318411_-1&amp;btsid=39551360-2e93-4fcf-b607-dc7a7b7ec915"/>
+    <hyperlink ref="G3" r:id="rId1" display="Stepper motor"/>
+    <hyperlink ref="G4" r:id="rId2" display="stepper motor driver search"/>
+    <hyperlink ref="G5" r:id="rId3" display="BTM-800 PRX"/>
+    <hyperlink ref="G6" r:id="rId4" display="PIR motion sensor"/>
+    <hyperlink ref="G7" r:id="rId5" display="PCX ble usb search"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated for new components
</commit_message>
<xml_diff>
--- a/price.xlsx
+++ b/price.xlsx
@@ -5,22 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="960" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Item</t>
   </si>
@@ -88,7 +83,16 @@
     <t>PI BLE</t>
   </si>
   <si>
-    <t>PCX ble usb search</t>
+    <t>König CSBLUEKEY200</t>
+  </si>
+  <si>
+    <t>http://www.euronics.hu/</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>HDMI-DVI</t>
   </si>
 </sst>
 </file>
@@ -229,10 +233,11 @@
   <dxfs count="1">
     <dxf>
       <font>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
         <name val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
       </font>
       <numFmt numFmtId="164" formatCode="#.00"/>
       <fill>
@@ -310,10 +315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -367,8 +372,14 @@
     <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
       <c r="F2" s="4"/>
       <c r="G2" s="2"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -395,11 +406,11 @@
       </c>
       <c r="I3" s="6" t="n">
         <f aca="false">SUM(F:F)</f>
-        <v>52.5137722419929</v>
+        <v>73.8589679715302</v>
       </c>
       <c r="J3" s="6" t="n">
         <f aca="false">SUM(100-(I3))</f>
-        <v>47.4862277580071</v>
+        <v>26.1410320284698</v>
       </c>
       <c r="N3" s="8" t="n">
         <v>281</v>
@@ -448,7 +459,7 @@
       </c>
       <c r="F5" s="6" t="n">
         <f aca="false">E5*(C5+D5)</f>
-        <v>37.7437722419929</v>
+        <v>37.7437722419928</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>17</v>
@@ -478,22 +489,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <f aca="false">2999/N3</f>
+        <v>10.6725978647687</v>
       </c>
       <c r="F7" s="6" t="n">
         <f aca="false">E7*(C7+D7)</f>
+        <v>10.6725978647687</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
+      <c r="E8" s="6" t="n">
+        <f aca="false">2999/N3</f>
+        <v>10.6725978647687</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <f aca="false">E8*(C8+D8)</f>
+        <v>10.6725978647687</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -507,7 +550,8 @@
     <hyperlink ref="G4" r:id="rId2" display="stepper motor driver search"/>
     <hyperlink ref="G5" r:id="rId3" display="BTM-800 PRX"/>
     <hyperlink ref="G6" r:id="rId4" display="PIR motion sensor"/>
-    <hyperlink ref="G7" r:id="rId5" display="PCX ble usb search"/>
+    <hyperlink ref="G7" r:id="rId5" display="http://www.euronics.hu/"/>
+    <hyperlink ref="G8" r:id="rId6" display="http://www.euronics.hu/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>